<commit_message>
Updated Excel to show how the algorithm works
</commit_message>
<xml_diff>
--- a/AlgoTest.xlsx
+++ b/AlgoTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Job\EnactOn\InterviewCode\laravel-interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5578BFFC-BB60-4C4B-A1D1-23CC54041F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC36810-463E-46E8-B62A-B33E1A6EDB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D3ED041D-8D72-4617-BC90-B9B83FA3C2A8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>a</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>Total Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prize Percent </t>
+  </si>
+  <si>
+    <t>Whole Numbers</t>
+  </si>
+  <si>
+    <t>Round 1 Distribution</t>
+  </si>
+  <si>
+    <t>Round 2 Distribution</t>
+  </si>
+  <si>
+    <t>Acutal Percent</t>
+  </si>
+  <si>
+    <t>Fractions</t>
+  </si>
+  <si>
+    <t>Sorting</t>
   </si>
 </sst>
 </file>
@@ -430,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E1B77C-FCE1-49C2-8F6D-E78764AA505E}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,17 +462,21 @@
     <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -947,6 +972,230 @@
         <v>100</v>
       </c>
     </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <f>C2</f>
+        <v>0.65</v>
+      </c>
+      <c r="G15">
+        <f>FLOOR(C2,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>G15</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>E15-G15</f>
+        <v>0.65</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <f>J15+P15</f>
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <f>E2</f>
+        <v>7.6923076923076925</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f>C3</f>
+        <v>1.3</v>
+      </c>
+      <c r="G16">
+        <f>FLOOR(C3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J20" si="3">G16</f>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <f>E16-G16</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f>J16+P16</f>
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <f>E3</f>
+        <v>7.6923076923076925</v>
+      </c>
+    </row>
+    <row r="17" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <f>C4</f>
+        <v>3.25</v>
+      </c>
+      <c r="G17">
+        <f>FLOOR(C4,1)</f>
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <f>E17-G17</f>
+        <v>0.25</v>
+      </c>
+      <c r="N17">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>J17+P17</f>
+        <v>3</v>
+      </c>
+      <c r="S17">
+        <f>E4</f>
+        <v>23.076923076923077</v>
+      </c>
+    </row>
+    <row r="18" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <f>C5</f>
+        <v>1.3</v>
+      </c>
+      <c r="G18">
+        <f>FLOOR(C5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <f>E18-G18</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f>J18+P18</f>
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <f>E5</f>
+        <v>7.6923076923076925</v>
+      </c>
+    </row>
+    <row r="19" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f>C6</f>
+        <v>3.9325000000000001</v>
+      </c>
+      <c r="G19">
+        <f>FLOOR(C6,1)</f>
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <f>E19-G19</f>
+        <v>0.93250000000000011</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <f>J19+P19</f>
+        <v>4</v>
+      </c>
+      <c r="S19">
+        <f>E6</f>
+        <v>30.76923076923077</v>
+      </c>
+    </row>
+    <row r="20" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <f>C7</f>
+        <v>2.5674999999999999</v>
+      </c>
+      <c r="G20">
+        <f>FLOOR(C7,1)</f>
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <f>E20-G20</f>
+        <v>0.56749999999999989</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <f>J20+P20</f>
+        <v>3</v>
+      </c>
+      <c r="S20">
+        <f>E7</f>
+        <v>23.076923076923077</v>
+      </c>
+    </row>
+    <row r="21" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="R21" s="1">
+        <f>SUM(R15:R20)</f>
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>